<commit_message>
commit persional word 6.27
</commit_message>
<xml_diff>
--- a/个人工作记录_柳云肖.xlsx
+++ b/个人工作记录_柳云肖.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>日期</t>
   </si>
@@ -261,12 +261,103 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>PHP 文件处理</t>
+    <t>PHP include 和 require 语句</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过 include 或 require 语句，可以将 PHP 文件的内容插入另一个 PHP 文件（在服务器执行它之前）。
+include 和 require 语句是相同的，除了错误处理方面：
+require 会生成致命错误（E_COMPILE_ERROR）并停止脚本
+include 只生成警告（E_WARNING），并且脚本会继续</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>因此，如果您希望继续执行，并向用户输出结果，即使包含文件已丢失，那么请使用 include。否则，在框架、CMS 或者复杂的 PHP 应用程序编程中，请始终使用 require 向执行流引用关键文件。这有助于提高应用程序的安全性和完整性，在某个关键文件意外丢失的情况下。
+包含文件省去了大量的工作。这意味着您可以为所有页面创建标准页头、页脚或者菜单文件。然后，在页头需要更新时，您只需更新这个页头包含文件即可。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>include 'filename';
+require 'filename';</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意：请谨慎操作文件！
+当您操作文件时必须非常小心。如果您操作失误，可能会造成非常严重的破坏。常见的错误是：
+编辑错误的文件
+被垃圾数据填满硬盘
+意外删除文件内容</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>PHP 操作文件</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 文件处理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP readfile() 函数
+readfile() 函数读取文件，并把它写入输出缓冲。如果您想做的所有事情就是打开一个文件并读取器内容，那么 readfile() 函数很有用。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 操作文件
+PHP 拥有的多种函数可供创建、读取、上传以及编辑文件。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 文件打开/读取/读取</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;?php
+$myfile = fopen("webdictionary.txt", "r") or die("Unable to open file!");
+echo fread($myfile,filesize("webdictionary.txt"));
+fclose($myfile);
+?&gt;
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP Open File - fopen()
+打开文件的更好的方法是通过 fopen() 函数。此函数为您提供比 readfile() 函数更多的选项。
+fopen() 的第一个参数包含被打开的文件名，第二个参数规定打开文件的模式。如果 fopen() 函数未能打开指定的文件，
+PHP 读取文件 - fread()
+fread() 函数读取打开的文件。
+fread() 的第一个参数包含待读取文件的文件名，第二个参数规定待读取的最大字节数。
+PHP 关闭文件 - fclose()
+fclose() 函数用于关闭打开的文件。
+注释：用完文件后把它们全部关闭是一个良好的编程习惯。您并不想打开的文件占用您的服务器资源。
+fclose() 需要待关闭文件的名称（或者存有文件名的变量）：
+PHP 读取单行文件 - fgets()
+fgets() 函数用于从文件读取单行。
+PHP 检查 End-Of-File - feof()
+feof() 函数检查是否已到达 "end-of-file" (EOF)。
+feof() 对于遍历未知长度的数据很有用。
+PHP 读取单字符 - fgetc()
+fgetc() 函数用于从文件中读取单个字符。
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PHP 创建文件 - fopen()
+fopen() 函数也用于创建文件。也许有点混乱，但是在 PHP 中，创建文件所用的函数与打开文件的相同。
+PHP 文件权限
+如果您试图运行这段代码时发生错误，请检查您是否有向硬盘写入信息的 PHP 文件访问权限。
+PHP 写入文件 - fwrite()
+fwrite() 函数用于写入文件。
+fwrite() 的第一个参数包含要写入的文件的文件名，第二个参数是被写的字符串。
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 文件创建/写入</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHP 文件上传</t>
   </si>
 </sst>
 </file>
@@ -421,7 +512,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -490,6 +581,15 @@
     </xf>
     <xf numFmtId="177" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -835,20 +935,20 @@
   <dimension ref="A1:G383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C168" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C175" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D173" sqref="D173"/>
+      <selection pane="bottomRight" activeCell="D180" sqref="D180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="2" width="8" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="34.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="73.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="32.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.75" style="4" customWidth="1"/>
+    <col min="6" max="6" width="64.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="32.875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -3374,17 +3474,17 @@
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="C173" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D173" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E173" s="8"/>
+      <c r="C173" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D173" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E173" s="20"/>
       <c r="F173" s="8"/>
       <c r="G173" s="9"/>
     </row>
-    <row r="174" spans="1:7" s="10" customFormat="1">
+    <row r="174" spans="1:7" s="10" customFormat="1" ht="175.5">
       <c r="A174" s="6">
         <v>42542</v>
       </c>
@@ -3392,13 +3492,21 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="C174" s="8"/>
-      <c r="D174" s="8"/>
-      <c r="E174" s="8"/>
-      <c r="F174" s="8"/>
-      <c r="G174" s="9"/>
-    </row>
-    <row r="175" spans="1:7" s="10" customFormat="1">
+      <c r="C174" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D174" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E174" s="18"/>
+      <c r="F174" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G174" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" s="10" customFormat="1" ht="81">
       <c r="A175" s="6">
         <v>42543</v>
       </c>
@@ -3406,13 +3514,18 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="C175" s="8"/>
-      <c r="D175" s="8"/>
-      <c r="E175" s="8"/>
-      <c r="F175" s="8"/>
-      <c r="G175" s="9"/>
-    </row>
-    <row r="176" spans="1:7" s="10" customFormat="1">
+      <c r="C175" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D175" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E175" s="18"/>
+      <c r="F175" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" s="10" customFormat="1" ht="297">
       <c r="A176" s="6">
         <v>42544</v>
       </c>
@@ -3420,13 +3533,19 @@
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="8"/>
-      <c r="E176" s="8"/>
-      <c r="F176" s="8"/>
+      <c r="C176" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D176" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E176" s="20"/>
+      <c r="F176" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="G176" s="9"/>
     </row>
-    <row r="177" spans="1:7" s="10" customFormat="1">
+    <row r="177" spans="1:7" s="10" customFormat="1" ht="135">
       <c r="A177" s="6">
         <v>42545</v>
       </c>
@@ -3434,8 +3553,12 @@
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="C177" s="8"/>
-      <c r="D177" s="8"/>
+      <c r="C177" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D177" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="E177" s="8"/>
       <c r="F177" s="8"/>
       <c r="G177" s="9"/>
@@ -3476,7 +3599,9 @@
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="C180" s="8"/>
+      <c r="C180" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="D180" s="8"/>
       <c r="E180" s="8"/>
       <c r="F180" s="8"/>

</xml_diff>